<commit_message>
Alwin Konstantin Agrippa (nad other stuff)
</commit_message>
<xml_diff>
--- a/Characters/Selanar Durothil/Campaign_Share/Party_Loot.xlsx
+++ b/Characters/Selanar Durothil/Campaign_Share/Party_Loot.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23229"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/eb9d5a2ad070901d/Role Playing Games/[D^0D] Dungeons ^0 Dragons/DnD_Character_Repository/Characters/Selanar Durothil/Campaign_Share/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/eb9d5a2ad070901d/Role Playing Games/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="952" documentId="8_{D438E813-1674-4A3A-A68B-B3E54D9D336A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{564F8F44-CAD8-4C74-A924-F063609FA92C}"/>
+  <xr:revisionPtr revIDLastSave="977" documentId="8_{D438E813-1674-4A3A-A68B-B3E54D9D336A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{1E6C1E7D-0544-4421-9399-6D49FB5F3499}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="503" windowWidth="28996" windowHeight="15794" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="30270" yWindow="2070" windowWidth="21600" windowHeight="11423" firstSheet="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ledger" sheetId="2" r:id="rId1"/>
     <sheet name="Current Pool" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191028" calcCompleted="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="167">
   <si>
     <t>Date</t>
   </si>
@@ -237,6 +237,9 @@
     <t>Carrakas, Paleth, Anna</t>
   </si>
   <si>
+    <t>Q5 of sewer lair</t>
+  </si>
+  <si>
     <t>Paleth</t>
   </si>
   <si>
@@ -276,9 +279,15 @@
     <t>Black cloak with [Xanathar] symbol</t>
   </si>
   <si>
+    <t>20 yds. of Glamerweave fine cloth</t>
+  </si>
+  <si>
     <t>Q7 chest</t>
   </si>
   <si>
+    <t>Very nice, ornate chest [of Preservation]</t>
+  </si>
+  <si>
     <t>2 lb. bars of Mithral (Manta Ray stamp)</t>
   </si>
   <si>
@@ -408,6 +417,27 @@
     <t>Saphire</t>
   </si>
   <si>
+    <t>Censer of Command Air Elemental</t>
+  </si>
+  <si>
+    <t>Ship</t>
+  </si>
+  <si>
+    <t>Rocco</t>
+  </si>
+  <si>
+    <t>Big pile of mundane stuff</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Big pile of coins</t>
+  </si>
+  <si>
+    <t>Party</t>
+  </si>
+  <si>
     <t>Name</t>
   </si>
   <si>
@@ -426,88 +456,61 @@
     <t>WEAPONS</t>
   </si>
   <si>
-    <t>1 lb.</t>
+    <t>ARMORS</t>
+  </si>
+  <si>
+    <t>MAGIC ITEMS</t>
+  </si>
+  <si>
+    <t>Bag of holding</t>
+  </si>
+  <si>
+    <t>Quiver of Ehlonna</t>
+  </si>
+  <si>
+    <t>Rope of Climbing</t>
+  </si>
+  <si>
+    <t>Horn of Silent Alert</t>
+  </si>
+  <si>
+    <t>Ring of Water Breathing</t>
+  </si>
+  <si>
+    <t>Chest of Preservation</t>
+  </si>
+  <si>
+    <t>MUNDANE ITEMS</t>
   </si>
   <si>
     <t>5 lb.</t>
   </si>
   <si>
-    <t>ARMORS</t>
+    <t>Fine Boots</t>
+  </si>
+  <si>
+    <t>6 lb.</t>
+  </si>
+  <si>
+    <t>VALUABLES</t>
+  </si>
+  <si>
+    <t>(Jewelry) A bracelet with several charms on it</t>
+  </si>
+  <si>
+    <t>(Jewelry) A brass orb etched with strange runes</t>
+  </si>
+  <si>
+    <t>(Jewelry) Golden tokens with wings on both sides</t>
+  </si>
+  <si>
+    <t>(Material) 10 lb Silver Bars</t>
   </si>
   <si>
     <t>10 lb.</t>
   </si>
   <si>
-    <t>MAGIC ITEMS</t>
-  </si>
-  <si>
-    <t>Flask of drow poison (DC 13)</t>
-  </si>
-  <si>
-    <t>Light Crossbow (Drow)</t>
-  </si>
-  <si>
-    <t>Chain shirt (Drow)</t>
-  </si>
-  <si>
-    <t>Bag of holding</t>
-  </si>
-  <si>
-    <t>Quiver of Ehlonna</t>
-  </si>
-  <si>
-    <t>Rope of Climbing</t>
-  </si>
-  <si>
-    <t>Horn of Silent Alert</t>
-  </si>
-  <si>
-    <t>Ring of Water Breathing</t>
-  </si>
-  <si>
-    <t>Chest of Preservation</t>
-  </si>
-  <si>
-    <t>Censer of Command Air Elemental</t>
-  </si>
-  <si>
-    <t>MUNDANE ITEMS</t>
-  </si>
-  <si>
-    <t>Fine Boots</t>
-  </si>
-  <si>
-    <t>6 lb.</t>
-  </si>
-  <si>
-    <t>VALUABLES</t>
-  </si>
-  <si>
-    <t>(Art) 4 Large Paintings</t>
-  </si>
-  <si>
-    <t>(Jewelry) A bracelet with several charms on it</t>
-  </si>
-  <si>
-    <t>(Jewelry) A brass orb etched with strange runes</t>
-  </si>
-  <si>
-    <t>(Jewelry) Golden ring</t>
-  </si>
-  <si>
-    <t>(Jewelry) Golden tokens with wings on both sides</t>
-  </si>
-  <si>
-    <t>(Jewelry) Heart-shaped pendant of gold</t>
-  </si>
-  <si>
-    <t>(Jewelry) Wedding ring</t>
-  </si>
-  <si>
-    <t>(Jewelry) Zhentarim ring</t>
-  </si>
-  <si>
-    <t>(Material) 10 lb Silver Bars</t>
+    <t>12 lbs used for silvering</t>
   </si>
   <si>
     <t>A vial of quicksilver</t>
@@ -516,59 +519,29 @@
     <t>TRADE GOODS</t>
   </si>
   <si>
-    <t>10 sq. yds of silk</t>
+    <t>CURRENCY</t>
+  </si>
+  <si>
+    <t>Copper</t>
+  </si>
+  <si>
+    <t>0.02 lb.</t>
+  </si>
+  <si>
+    <t>Silver</t>
   </si>
   <si>
     <t>Gold</t>
   </si>
   <si>
     <t>Platinum</t>
-  </si>
-  <si>
-    <t>CURRENCY</t>
-  </si>
-  <si>
-    <t>Copper</t>
-  </si>
-  <si>
-    <t>0.02 lb.</t>
-  </si>
-  <si>
-    <t>Silver</t>
-  </si>
-  <si>
-    <t>Q5 of sewer lair</t>
-  </si>
-  <si>
-    <t>20 yds. of Glamerweave fine cloth</t>
-  </si>
-  <si>
-    <t>Very nice, ornate chest [of Preservation]</t>
-  </si>
-  <si>
-    <t>Ship</t>
-  </si>
-  <si>
-    <t>Rocco</t>
-  </si>
-  <si>
-    <t>Big pile of mundane stuff</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>Big pile of coins</t>
-  </si>
-  <si>
-    <t>Party</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -633,7 +606,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -653,16 +626,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -675,6 +639,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -955,30 +925,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F796F98-EF2E-4EE2-A45A-D67B29E359C1}">
-  <dimension ref="A1:E127"/>
+  <dimension ref="A1:E128"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D140" sqref="D140"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A106" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F128" sqref="F128"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="10.1328125" customWidth="1"/>
-    <col min="2" max="2" width="47.1328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.06640625" style="1"/>
-    <col min="4" max="4" width="16.265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="44.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" customWidth="1"/>
+    <col min="2" max="2" width="47.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9" style="1"/>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="44.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="18" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
@@ -988,7 +958,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5">
       <c r="B2" t="s">
         <v>5</v>
       </c>
@@ -1002,7 +972,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5">
       <c r="B3" t="s">
         <v>8</v>
       </c>
@@ -1016,7 +986,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5">
       <c r="B4" t="s">
         <v>9</v>
       </c>
@@ -1030,7 +1000,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5">
       <c r="B5" t="s">
         <v>10</v>
       </c>
@@ -1044,7 +1014,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5">
       <c r="B6" t="s">
         <v>11</v>
       </c>
@@ -1058,7 +1028,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5">
       <c r="B7" t="s">
         <v>12</v>
       </c>
@@ -1072,7 +1042,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5">
       <c r="B8" t="s">
         <v>13</v>
       </c>
@@ -1086,7 +1056,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:5">
       <c r="B9" t="s">
         <v>14</v>
       </c>
@@ -1100,7 +1070,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:5">
       <c r="B10" t="s">
         <v>15</v>
       </c>
@@ -1114,7 +1084,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:5">
       <c r="B11" t="s">
         <v>16</v>
       </c>
@@ -1128,7 +1098,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:5">
       <c r="B12" t="s">
         <v>17</v>
       </c>
@@ -1142,7 +1112,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:5">
       <c r="B13" t="s">
         <v>18</v>
       </c>
@@ -1156,7 +1126,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:5">
       <c r="B14" t="s">
         <v>19</v>
       </c>
@@ -1170,7 +1140,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:5">
       <c r="B15" t="s">
         <v>20</v>
       </c>
@@ -1184,7 +1154,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:5">
       <c r="B16" t="s">
         <v>21</v>
       </c>
@@ -1198,7 +1168,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:5">
       <c r="B17" t="s">
         <v>22</v>
       </c>
@@ -1212,7 +1182,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:5">
       <c r="B18" t="s">
         <v>23</v>
       </c>
@@ -1226,7 +1196,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:5">
       <c r="B19" t="s">
         <v>24</v>
       </c>
@@ -1240,7 +1210,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:5">
       <c r="B20" t="s">
         <v>25</v>
       </c>
@@ -1254,7 +1224,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:5">
       <c r="B21" t="s">
         <v>26</v>
       </c>
@@ -1268,7 +1238,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:5">
       <c r="B22" t="s">
         <v>27</v>
       </c>
@@ -1282,7 +1252,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:5">
       <c r="B23" t="s">
         <v>28</v>
       </c>
@@ -1296,7 +1266,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:5">
       <c r="B24" t="s">
         <v>29</v>
       </c>
@@ -1310,7 +1280,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:5">
       <c r="B25" t="s">
         <v>30</v>
       </c>
@@ -1324,7 +1294,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:5">
       <c r="B26" t="s">
         <v>31</v>
       </c>
@@ -1338,7 +1308,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:5">
       <c r="B27" t="s">
         <v>32</v>
       </c>
@@ -1352,7 +1322,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:5">
       <c r="A28" s="7">
         <v>44023</v>
       </c>
@@ -1369,8 +1339,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A29" s="11">
+    <row r="29" spans="1:5" s="5" customFormat="1">
+      <c r="A29" s="9">
         <v>44023</v>
       </c>
       <c r="B29" s="5" t="s">
@@ -1386,7 +1356,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:5">
       <c r="A30" s="7">
         <v>44023</v>
       </c>
@@ -1403,7 +1373,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:5">
       <c r="A31" s="7">
         <v>44023</v>
       </c>
@@ -1420,7 +1390,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:5">
       <c r="A32" s="7">
         <v>44023</v>
       </c>
@@ -1437,8 +1407,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A33" s="11">
+    <row r="33" spans="1:5" s="5" customFormat="1">
+      <c r="A33" s="9">
         <v>44023</v>
       </c>
       <c r="B33" s="5" t="s">
@@ -1454,7 +1424,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:5">
       <c r="A34" s="7">
         <v>44023</v>
       </c>
@@ -1471,7 +1441,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:5">
       <c r="A35" s="7">
         <v>44023</v>
       </c>
@@ -1488,7 +1458,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:5">
       <c r="A36" s="7">
         <v>44023</v>
       </c>
@@ -1505,7 +1475,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:5">
       <c r="A37" s="7">
         <v>44023</v>
       </c>
@@ -1522,7 +1492,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:5">
       <c r="A38" s="7">
         <v>44023</v>
       </c>
@@ -1539,7 +1509,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:5">
       <c r="A39" s="7">
         <v>44023</v>
       </c>
@@ -1556,7 +1526,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:5">
       <c r="A40" s="7">
         <v>44023</v>
       </c>
@@ -1573,7 +1543,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:5">
       <c r="A41" s="7">
         <v>44023</v>
       </c>
@@ -1590,7 +1560,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:5">
       <c r="A42" s="7">
         <v>44023</v>
       </c>
@@ -1607,7 +1577,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:5">
       <c r="A43" s="7">
         <v>44023</v>
       </c>
@@ -1624,7 +1594,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:5">
       <c r="A44" s="7">
         <v>44023</v>
       </c>
@@ -1641,7 +1611,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:5">
       <c r="A45" s="7">
         <v>44023</v>
       </c>
@@ -1658,7 +1628,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:5">
       <c r="A46" s="7">
         <v>44023</v>
       </c>
@@ -1672,7 +1642,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:5">
       <c r="A47" s="7">
         <v>44023</v>
       </c>
@@ -1686,7 +1656,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:5">
       <c r="A48" s="7">
         <v>44023</v>
       </c>
@@ -1700,7 +1670,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:5">
       <c r="A49" s="7">
         <v>44023</v>
       </c>
@@ -1714,7 +1684,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:5">
       <c r="A50" s="7">
         <v>44023</v>
       </c>
@@ -1728,7 +1698,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:5">
       <c r="A51" s="7">
         <v>44023</v>
       </c>
@@ -1742,7 +1712,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:5">
       <c r="A52" s="7">
         <v>44023</v>
       </c>
@@ -1756,7 +1726,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:5">
       <c r="A53" s="7">
         <v>44023</v>
       </c>
@@ -1770,7 +1740,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:5">
       <c r="A54" s="7">
         <v>44023</v>
       </c>
@@ -1784,7 +1754,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:5">
       <c r="A55" s="7">
         <v>44023</v>
       </c>
@@ -1798,7 +1768,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:5">
       <c r="A56" s="7">
         <v>44023</v>
       </c>
@@ -1812,7 +1782,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:5">
       <c r="A57" s="7">
         <v>44023</v>
       </c>
@@ -1826,7 +1796,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:5">
       <c r="A58" s="7">
         <v>44023</v>
       </c>
@@ -1840,8 +1810,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="59" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A59" s="11">
+    <row r="59" spans="1:5" s="5" customFormat="1">
+      <c r="A59" s="9">
         <v>44035</v>
       </c>
       <c r="B59" s="5" t="s">
@@ -1857,8 +1827,8 @@
         <v>65</v>
       </c>
     </row>
-    <row r="60" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A60" s="11">
+    <row r="60" spans="1:5" s="5" customFormat="1">
+      <c r="A60" s="9">
         <v>44036</v>
       </c>
       <c r="B60" s="5" t="s">
@@ -1874,8 +1844,8 @@
         <v>66</v>
       </c>
     </row>
-    <row r="61" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A61" s="11">
+    <row r="61" spans="1:5" s="5" customFormat="1">
+      <c r="A61" s="9">
         <v>44037</v>
       </c>
       <c r="B61" s="5" t="s">
@@ -1891,7 +1861,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:5">
       <c r="A62" s="7">
         <v>44038</v>
       </c>
@@ -1902,14 +1872,14 @@
         <v>2</v>
       </c>
       <c r="D62" t="s">
-        <v>167</v>
+        <v>67</v>
       </c>
       <c r="E62" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A63" s="11">
+    <row r="63" spans="1:5" s="5" customFormat="1">
+      <c r="A63" s="9">
         <v>44038</v>
       </c>
       <c r="B63" s="5" t="s">
@@ -1919,13 +1889,13 @@
         <v>1</v>
       </c>
       <c r="D63" t="s">
-        <v>167</v>
+        <v>67</v>
       </c>
       <c r="E63" s="5" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.45">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
       <c r="A64" s="7">
         <v>44038</v>
       </c>
@@ -1936,13 +1906,13 @@
         <v>6</v>
       </c>
       <c r="D64" t="s">
-        <v>167</v>
+        <v>67</v>
       </c>
       <c r="E64" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:5">
       <c r="A65" s="7">
         <v>44038</v>
       </c>
@@ -1953,81 +1923,81 @@
         <v>1</v>
       </c>
       <c r="D65" t="s">
-        <v>167</v>
+        <v>67</v>
       </c>
       <c r="E65" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:5">
       <c r="A66" s="7">
         <v>44038</v>
       </c>
       <c r="B66" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C66" s="1">
         <v>2</v>
       </c>
       <c r="D66" t="s">
-        <v>167</v>
+        <v>67</v>
       </c>
       <c r="E66" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:5">
       <c r="A67" s="7">
         <v>44038</v>
       </c>
       <c r="B67" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C67" s="1">
         <v>1</v>
       </c>
       <c r="D67" t="s">
-        <v>167</v>
+        <v>67</v>
       </c>
       <c r="E67" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:5">
       <c r="A68" s="7">
         <v>44038</v>
       </c>
       <c r="B68" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C68" s="1">
         <v>2</v>
       </c>
       <c r="D68" t="s">
-        <v>167</v>
+        <v>67</v>
       </c>
       <c r="E68" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:5">
       <c r="A69" s="7">
         <v>44038</v>
       </c>
       <c r="B69" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C69" s="1">
         <v>4</v>
       </c>
       <c r="D69" t="s">
-        <v>167</v>
+        <v>67</v>
       </c>
       <c r="E69" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:5">
       <c r="A70" s="7">
         <v>44038</v>
       </c>
@@ -2038,81 +2008,81 @@
         <v>3</v>
       </c>
       <c r="D70" t="s">
-        <v>167</v>
+        <v>67</v>
       </c>
       <c r="E70" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:5">
       <c r="A71" s="7">
         <v>44038</v>
       </c>
       <c r="B71" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C71" s="1">
         <v>2</v>
       </c>
       <c r="D71" t="s">
-        <v>167</v>
+        <v>67</v>
       </c>
       <c r="E71" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:5">
       <c r="A72" s="7">
         <v>44038</v>
       </c>
       <c r="B72" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C72" s="1">
         <v>1</v>
       </c>
       <c r="D72" t="s">
-        <v>167</v>
+        <v>67</v>
       </c>
       <c r="E72" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:5">
       <c r="A73" s="7">
         <v>44038</v>
       </c>
       <c r="B73" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C73" s="1">
         <v>1</v>
       </c>
       <c r="D73" t="s">
-        <v>167</v>
+        <v>67</v>
       </c>
       <c r="E73" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:5">
       <c r="A74" s="7">
         <v>44038</v>
       </c>
       <c r="B74" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C74" s="1">
         <v>4</v>
       </c>
       <c r="D74" t="s">
-        <v>167</v>
+        <v>67</v>
       </c>
       <c r="E74" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:5">
       <c r="A75" s="7">
         <v>44038</v>
       </c>
@@ -2123,30 +2093,30 @@
         <v>32</v>
       </c>
       <c r="D75" t="s">
-        <v>167</v>
+        <v>67</v>
       </c>
       <c r="E75" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:5">
       <c r="A76" s="7">
         <v>44038</v>
       </c>
       <c r="B76" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C76" s="1">
         <v>1</v>
       </c>
       <c r="D76" t="s">
-        <v>167</v>
+        <v>67</v>
       </c>
       <c r="E76" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:5">
       <c r="A77" s="7">
         <v>44038</v>
       </c>
@@ -2157,64 +2127,64 @@
         <v>2</v>
       </c>
       <c r="D77" t="s">
-        <v>167</v>
+        <v>67</v>
       </c>
       <c r="E77" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:5">
       <c r="A78" s="7">
         <v>44038</v>
       </c>
       <c r="B78" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C78" s="1">
         <v>1</v>
       </c>
       <c r="D78" t="s">
-        <v>167</v>
+        <v>67</v>
       </c>
       <c r="E78" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:5">
       <c r="A79" s="7">
         <v>44038</v>
       </c>
       <c r="B79" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C79" s="1">
         <v>2</v>
       </c>
       <c r="D79" t="s">
-        <v>167</v>
+        <v>67</v>
       </c>
       <c r="E79" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:5">
       <c r="A80" s="7">
         <v>44038</v>
       </c>
       <c r="B80" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C80" s="1">
         <v>3</v>
       </c>
       <c r="D80" t="s">
-        <v>167</v>
+        <v>67</v>
       </c>
       <c r="E80" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:5">
       <c r="A81" s="7">
         <v>44038</v>
       </c>
@@ -2225,421 +2195,421 @@
         <v>6</v>
       </c>
       <c r="D81" t="s">
-        <v>167</v>
+        <v>67</v>
       </c>
       <c r="E81" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:5">
       <c r="A82" s="7">
         <v>44038</v>
       </c>
       <c r="B82" t="s">
-        <v>168</v>
+        <v>81</v>
       </c>
       <c r="C82" s="1">
         <v>1</v>
       </c>
       <c r="D82" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E82" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:5">
       <c r="A83" s="7">
         <v>44038</v>
       </c>
       <c r="B83" t="s">
-        <v>169</v>
+        <v>83</v>
       </c>
       <c r="C83" s="1">
         <v>1</v>
       </c>
       <c r="D83" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E83" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A84" s="11">
+    <row r="84" spans="1:5">
+      <c r="A84" s="9">
         <v>44038</v>
       </c>
       <c r="B84" s="5" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C84" s="6">
         <v>5</v>
       </c>
       <c r="D84" s="5" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E84" s="5" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.45">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5">
       <c r="A85" s="7">
         <v>44038</v>
       </c>
       <c r="B85" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C85" s="1">
         <v>4</v>
       </c>
       <c r="D85" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E85" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="86" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A86" s="11">
+    <row r="86" spans="1:5" s="5" customFormat="1">
+      <c r="A86" s="9">
         <v>44038</v>
       </c>
       <c r="B86" s="5" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C86" s="6">
         <v>1</v>
       </c>
       <c r="D86" s="5" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E86" s="5" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A87" s="11">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" s="5" customFormat="1">
+      <c r="A87" s="9">
         <v>44038</v>
       </c>
       <c r="B87" s="5" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="C87" s="6">
         <v>1</v>
       </c>
       <c r="D87" s="5" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E87" s="5" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.45">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5">
       <c r="A88" s="7">
         <v>44038</v>
       </c>
       <c r="B88" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="C88" s="1">
         <v>1</v>
       </c>
       <c r="D88" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E88" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:5">
       <c r="A89" s="7">
         <v>44038</v>
       </c>
       <c r="B89" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="C89" s="1">
         <v>1</v>
       </c>
       <c r="D89" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E89" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="90" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A90" s="11">
+    <row r="90" spans="1:5" s="5" customFormat="1">
+      <c r="A90" s="9">
         <v>44038</v>
       </c>
       <c r="B90" s="5" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="C90" s="6">
         <v>1</v>
       </c>
       <c r="D90" s="5" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E90" s="5" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.45">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5">
       <c r="A91" s="7">
         <v>44039</v>
       </c>
       <c r="B91" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="C91" s="1">
         <v>1</v>
       </c>
       <c r="D91" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E91" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A92" s="11">
+    <row r="92" spans="1:5">
+      <c r="A92" s="9">
         <v>44038</v>
       </c>
       <c r="B92" s="5" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C92" s="6">
         <v>5</v>
       </c>
       <c r="D92" s="5" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E92" s="5" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A93" s="11">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5">
+      <c r="A93" s="9">
         <v>44038</v>
       </c>
       <c r="B93" s="5" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="C93" s="6">
         <v>1</v>
       </c>
       <c r="D93" s="5" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="E93" s="5" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A94" s="11">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5">
+      <c r="A94" s="9">
         <v>44038</v>
       </c>
       <c r="B94" s="5" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="C94" s="6">
         <v>1</v>
       </c>
       <c r="D94" s="5" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="E94" s="5" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.45">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5">
       <c r="A95" s="7">
         <v>44038</v>
       </c>
       <c r="B95" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="C95" s="1">
         <v>1</v>
       </c>
       <c r="D95" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="E95" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:5">
       <c r="A96" s="7">
         <v>44038</v>
       </c>
       <c r="B96" t="s">
+        <v>100</v>
+      </c>
+      <c r="C96" s="1">
+        <v>1</v>
+      </c>
+      <c r="D96" t="s">
         <v>97</v>
       </c>
-      <c r="C96" s="1">
-        <v>1</v>
-      </c>
-      <c r="D96" t="s">
-        <v>94</v>
-      </c>
       <c r="E96" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:5">
       <c r="A97" s="7">
         <v>44044</v>
       </c>
       <c r="B97" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="C97" s="1">
         <v>1</v>
       </c>
       <c r="D97" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="E97" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:5">
       <c r="A98" s="7">
         <v>44044</v>
       </c>
       <c r="B98" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="C98" s="1">
         <v>1</v>
       </c>
       <c r="D98" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="E98" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:5">
       <c r="A99" s="7">
         <v>44044</v>
       </c>
       <c r="B99" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="C99" s="1">
         <v>1</v>
       </c>
       <c r="D99" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="E99" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:5">
       <c r="A100" s="7">
         <v>44044</v>
       </c>
       <c r="B100" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="C100" s="1">
         <v>1</v>
       </c>
       <c r="D100" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="E100" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:5">
       <c r="A101" s="7">
         <v>44044</v>
       </c>
       <c r="B101" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="C101" s="1">
         <v>20</v>
       </c>
       <c r="D101" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="E101" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:5">
       <c r="A102" s="7">
         <v>44044</v>
       </c>
       <c r="B102" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="C102" s="1">
         <v>1</v>
       </c>
       <c r="D102" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="E102" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:5">
       <c r="A103" s="7">
         <v>44044</v>
       </c>
       <c r="B103" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="C103" s="1">
         <v>1</v>
       </c>
       <c r="D103" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="E103" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="104" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A104" s="11">
+    <row r="104" spans="1:5" s="5" customFormat="1">
+      <c r="A104" s="9">
         <v>44044</v>
       </c>
       <c r="B104" s="5" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C104" s="6">
         <v>1</v>
       </c>
       <c r="D104" s="5" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="E104" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A105" s="11">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" s="5" customFormat="1">
+      <c r="A105" s="9">
         <v>44044</v>
       </c>
       <c r="B105" s="5" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="C105" s="6">
         <v>1</v>
       </c>
       <c r="D105" s="5" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="E105" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.45">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5">
       <c r="A106" s="7">
         <v>44044</v>
       </c>
@@ -2650,47 +2620,47 @@
         <v>50</v>
       </c>
       <c r="D106" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="E106" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:5">
       <c r="A107" s="7">
         <v>44044</v>
       </c>
       <c r="B107" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="C107" s="1">
         <v>2</v>
       </c>
       <c r="D107" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="E107" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:5">
       <c r="A108" s="7">
         <v>44044</v>
       </c>
       <c r="B108" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="C108" s="1">
         <v>2</v>
       </c>
       <c r="D108" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="E108" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:5">
       <c r="A109" s="7">
         <v>44044</v>
       </c>
@@ -2701,30 +2671,30 @@
         <v>16</v>
       </c>
       <c r="D109" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="E109" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:5">
       <c r="A110" s="7">
         <v>44044</v>
       </c>
       <c r="B110" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="C110" s="1">
         <v>2</v>
       </c>
       <c r="D110" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="E110" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:5">
       <c r="A111" s="7">
         <v>44044</v>
       </c>
@@ -2735,218 +2705,218 @@
         <v>2</v>
       </c>
       <c r="D111" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="E111" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:5">
       <c r="A112" s="7">
         <v>44044</v>
       </c>
       <c r="B112" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="C112" s="1">
         <v>1</v>
       </c>
       <c r="D112" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="E112" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:5">
       <c r="A113" s="7">
         <v>44044</v>
       </c>
       <c r="B113" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C113" s="1">
         <v>1</v>
       </c>
       <c r="D113" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="E113" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:5">
       <c r="A114" s="7">
         <v>44044</v>
       </c>
       <c r="B114" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="C114" s="1">
         <v>1</v>
       </c>
       <c r="D114" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="E114" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:5">
       <c r="A115" s="7">
         <v>44044</v>
       </c>
       <c r="B115" t="s">
+        <v>118</v>
+      </c>
+      <c r="C115" s="1">
+        <v>1</v>
+      </c>
+      <c r="D115" t="s">
         <v>115</v>
       </c>
-      <c r="C115" s="1">
-        <v>1</v>
-      </c>
-      <c r="D115" t="s">
-        <v>112</v>
-      </c>
       <c r="E115" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:5">
       <c r="A116" s="7">
         <v>44044</v>
       </c>
       <c r="B116" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="C116" s="1">
         <v>1</v>
       </c>
       <c r="D116" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="E116" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:5">
       <c r="A117" s="7">
         <v>44044</v>
       </c>
       <c r="B117" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="C117" s="1">
         <v>1</v>
       </c>
       <c r="D117" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="E117" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:5">
       <c r="A118" s="7">
         <v>44044</v>
       </c>
       <c r="B118" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="C118" s="1">
         <v>1</v>
       </c>
       <c r="D118" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="E118" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:5">
       <c r="A119" s="7">
         <v>44044</v>
       </c>
       <c r="B119" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="C119" s="1">
         <v>3</v>
       </c>
       <c r="D119" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="E119" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:5">
       <c r="A120" s="7">
         <v>44044</v>
       </c>
       <c r="B120" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="C120" s="1">
         <v>1</v>
       </c>
       <c r="D120" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="E120" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="121" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A121" s="13">
+    <row r="121" spans="1:5" s="11" customFormat="1">
+      <c r="A121" s="10">
         <v>44044</v>
       </c>
-      <c r="B121" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="C121" s="16">
-        <v>1</v>
-      </c>
-      <c r="D121" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="E121" s="14" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B121" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="C121" s="13">
+        <v>1</v>
+      </c>
+      <c r="D121" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="E121" s="11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5">
       <c r="A122" s="7">
         <v>44044</v>
       </c>
       <c r="B122" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="C122" s="1">
         <v>1</v>
       </c>
       <c r="D122" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="E122" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:5">
       <c r="A123" s="7">
         <v>44044</v>
       </c>
       <c r="B123" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="C123" s="1">
         <v>1</v>
       </c>
       <c r="D123" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="E123" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="124" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A124" s="11">
+    <row r="124" spans="1:5" s="5" customFormat="1">
+      <c r="A124" s="9">
         <v>44044</v>
       </c>
       <c r="B124" s="5" t="s">
@@ -2959,58 +2929,75 @@
         <v>7</v>
       </c>
       <c r="E124" s="5" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="125" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A125" s="11">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" s="5" customFormat="1">
+      <c r="A125" s="9">
         <v>44044</v>
       </c>
       <c r="B125" s="5" t="s">
-        <v>144</v>
+        <v>127</v>
       </c>
       <c r="C125" s="6">
         <v>1</v>
       </c>
       <c r="D125" s="5" t="s">
-        <v>170</v>
+        <v>128</v>
       </c>
       <c r="E125" s="5" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="126" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A126" s="11">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" s="5" customFormat="1">
+      <c r="A126" s="9">
         <v>44044</v>
       </c>
       <c r="B126" s="5" t="s">
-        <v>172</v>
+        <v>130</v>
       </c>
       <c r="C126" s="6" t="s">
-        <v>173</v>
+        <v>131</v>
       </c>
       <c r="D126" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E126" s="5" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="127" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A127" s="11">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" s="5" customFormat="1">
+      <c r="A127" s="9">
         <v>44044</v>
       </c>
       <c r="B127" s="5" t="s">
-        <v>174</v>
+        <v>132</v>
       </c>
       <c r="C127" s="6" t="s">
-        <v>173</v>
+        <v>131</v>
       </c>
       <c r="D127" s="5" t="s">
-        <v>171</v>
+        <v>129</v>
       </c>
       <c r="E127" s="5" t="s">
-        <v>175</v>
+        <v>133</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5">
+      <c r="A128" s="7">
+        <v>44079</v>
+      </c>
+      <c r="B128" t="s">
+        <v>86</v>
+      </c>
+      <c r="C128" s="1">
+        <v>5</v>
+      </c>
+      <c r="D128" t="s">
+        <v>129</v>
+      </c>
+      <c r="E128" t="s">
+        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -3021,669 +3008,577 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I127"/>
+  <dimension ref="A1:I117"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P12" sqref="P12"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D59" sqref="D59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="42.86328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" style="1"/>
     <col min="3" max="3" width="14" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.46484375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.265625" customWidth="1"/>
+    <col min="6" max="6" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>126</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>127</v>
+    <row r="1" spans="1:7" s="2" customFormat="1">
+      <c r="A1" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>135</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>137</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A2" s="12" t="s">
-        <v>129</v>
-      </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+    </row>
+    <row r="4" spans="1:7">
       <c r="C4" s="8"/>
-      <c r="G4" s="15"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="G5" s="15"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="G6" s="15"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="G7" s="15"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="G8" s="15"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="G9" s="15"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="G10" s="15"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="G11" s="15"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="G12" s="15"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="G13" s="15"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A16" s="12" t="s">
-        <v>132</v>
-      </c>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A17" s="9"/>
-      <c r="B17" s="9"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A23" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="B23" s="12"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A24" s="9"/>
-      <c r="B24" s="9"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="9"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="G4" s="12"/>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="G5" s="12"/>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="G6" s="12"/>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="G7" s="12"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="G8" s="12"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="G9" s="12"/>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="G10" s="12"/>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="G11" s="12"/>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="G12" s="12"/>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="G13" s="12"/>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="18"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="B23" s="19"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="19"/>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24" s="18"/>
+      <c r="B24" s="18"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+    </row>
+    <row r="25" spans="1:9">
       <c r="A25" t="s">
-        <v>135</v>
+        <v>40</v>
       </c>
       <c r="B25" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" s="11" customFormat="1">
+      <c r="A26" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="B26" s="15">
+        <v>1</v>
+      </c>
+      <c r="C26" s="15"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="14"/>
+      <c r="I26" s="14" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" s="11" customFormat="1">
+      <c r="A27" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="B27" s="15">
+        <v>1</v>
+      </c>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="14"/>
+      <c r="I27" s="14" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" s="11" customFormat="1">
+      <c r="A28" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="B28" s="13">
+        <v>1</v>
+      </c>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+    </row>
+    <row r="29" spans="1:9" s="11" customFormat="1">
+      <c r="A29" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="B29" s="13">
+        <v>1</v>
+      </c>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+    </row>
+    <row r="30" spans="1:9" s="11" customFormat="1">
+      <c r="A30" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="B30" s="15">
+        <v>1</v>
+      </c>
+      <c r="C30" s="15"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="14"/>
+      <c r="G30" s="14"/>
+      <c r="H30" s="14"/>
+      <c r="I30" s="14" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="A31" t="s">
+        <v>147</v>
+      </c>
+      <c r="B31" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="19" t="s">
+        <v>148</v>
+      </c>
+      <c r="B35" s="19"/>
+      <c r="C35" s="19"/>
+      <c r="D35" s="19"/>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" t="s">
+        <v>21</v>
+      </c>
+      <c r="B37" s="1">
         <v>2</v>
       </c>
-      <c r="C25" s="1">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A26" t="s">
-        <v>40</v>
-      </c>
-      <c r="B26" s="1">
+      <c r="C37" s="1">
+        <v>2</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" t="s">
+        <v>80</v>
+      </c>
+      <c r="B38" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" t="s">
+        <v>25</v>
+      </c>
+      <c r="B39" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" t="s">
+        <v>24</v>
+      </c>
+      <c r="B40" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" t="s">
+        <v>100</v>
+      </c>
+      <c r="B41" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" t="s">
+        <v>150</v>
+      </c>
+      <c r="B42" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" t="s">
+        <v>99</v>
+      </c>
+      <c r="B43" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" t="s">
+        <v>20</v>
+      </c>
+      <c r="B44" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" t="s">
+        <v>22</v>
+      </c>
+      <c r="B45" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" t="s">
+        <v>23</v>
+      </c>
+      <c r="B46" s="1">
+        <v>2</v>
+      </c>
+      <c r="C46" s="1">
+        <v>2</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" t="s">
+        <v>74</v>
+      </c>
+      <c r="B47" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" t="s">
+        <v>19</v>
+      </c>
+      <c r="B48" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" t="s">
+        <v>77</v>
+      </c>
+      <c r="B49" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" t="s">
+        <v>101</v>
+      </c>
+      <c r="B50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" t="s">
+        <v>102</v>
+      </c>
+      <c r="B51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" t="s">
+        <v>103</v>
+      </c>
+      <c r="B52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" t="s">
+        <v>106</v>
+      </c>
+      <c r="B53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" t="s">
+        <v>107</v>
+      </c>
+      <c r="B54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" s="19" t="s">
+        <v>152</v>
+      </c>
+      <c r="B60" s="19"/>
+      <c r="C60" s="19"/>
+      <c r="D60" s="19"/>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62" t="s">
+        <v>153</v>
+      </c>
+      <c r="B62" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63" t="s">
+        <v>154</v>
+      </c>
+      <c r="B63" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64" t="s">
+        <v>155</v>
+      </c>
+      <c r="B64" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9">
+      <c r="A65" t="s">
+        <v>156</v>
+      </c>
+      <c r="B65" s="1">
+        <v>6</v>
+      </c>
+      <c r="C65" s="1">
+        <v>50</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="I65" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9">
+      <c r="A66" t="s">
+        <v>47</v>
+      </c>
+      <c r="B66" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9">
+      <c r="A67" t="s">
+        <v>42</v>
+      </c>
+      <c r="B67" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9">
+      <c r="A68" t="s">
+        <v>159</v>
+      </c>
+      <c r="B68" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9">
+      <c r="A69" t="s">
+        <v>48</v>
+      </c>
+      <c r="B69" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9">
+      <c r="B71"/>
+    </row>
+    <row r="73" spans="1:9">
+      <c r="B73"/>
+    </row>
+    <row r="75" spans="1:9">
+      <c r="B75"/>
+    </row>
+    <row r="77" spans="1:9">
+      <c r="B77"/>
+    </row>
+    <row r="78" spans="1:9">
+      <c r="B78"/>
+    </row>
+    <row r="79" spans="1:9">
+      <c r="B79"/>
+    </row>
+    <row r="81" spans="1:4">
+      <c r="B81"/>
+    </row>
+    <row r="82" spans="1:4">
+      <c r="B82"/>
+    </row>
+    <row r="83" spans="1:4">
+      <c r="B83"/>
+    </row>
+    <row r="84" spans="1:4">
+      <c r="B84"/>
+    </row>
+    <row r="85" spans="1:4">
+      <c r="B85"/>
+    </row>
+    <row r="86" spans="1:4">
+      <c r="B86"/>
+    </row>
+    <row r="91" spans="1:4">
+      <c r="A91" s="19" t="s">
+        <v>160</v>
+      </c>
+      <c r="B91" s="19"/>
+      <c r="C91" s="19"/>
+      <c r="D91" s="19"/>
+    </row>
+    <row r="111" spans="1:4">
+      <c r="A111" s="19" t="s">
+        <v>161</v>
+      </c>
+      <c r="B111" s="19"/>
+      <c r="C111" s="19"/>
+      <c r="D111" s="19"/>
+    </row>
+    <row r="113" spans="1:6">
+      <c r="A113" t="s">
+        <v>162</v>
+      </c>
+      <c r="B113" s="1">
+        <v>2</v>
+      </c>
+      <c r="C113" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="D113" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="F113">
+        <f>B113*C113</f>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6">
+      <c r="A114" t="s">
+        <v>164</v>
+      </c>
+      <c r="B114" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A27" t="s">
-        <v>136</v>
-      </c>
-      <c r="B27" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A28" t="s">
-        <v>137</v>
-      </c>
-      <c r="B28" s="1">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A29" s="17" t="s">
-        <v>138</v>
-      </c>
-      <c r="B29" s="18">
-        <v>1</v>
-      </c>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="17"/>
-      <c r="F29" s="17"/>
-      <c r="G29" s="17"/>
-      <c r="H29" s="17"/>
-      <c r="I29" s="17" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A30" s="17" t="s">
-        <v>139</v>
-      </c>
-      <c r="B30" s="18">
-        <v>1</v>
-      </c>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="17"/>
-      <c r="F30" s="17"/>
-      <c r="G30" s="17"/>
-      <c r="H30" s="17"/>
-      <c r="I30" s="17" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A31" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="B31" s="16">
-        <v>1</v>
-      </c>
-      <c r="C31" s="16"/>
-      <c r="D31" s="16"/>
-    </row>
-    <row r="32" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A32" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="B32" s="16">
-        <v>1</v>
-      </c>
-      <c r="C32" s="16"/>
-      <c r="D32" s="16"/>
-    </row>
-    <row r="33" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A33" s="17" t="s">
-        <v>142</v>
-      </c>
-      <c r="B33" s="18">
-        <v>1</v>
-      </c>
-      <c r="C33" s="18"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="17"/>
-      <c r="F33" s="17"/>
-      <c r="G33" s="17"/>
-      <c r="H33" s="17"/>
-      <c r="I33" s="17" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A34" t="s">
-        <v>143</v>
-      </c>
-      <c r="B34" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A38" s="12" t="s">
-        <v>145</v>
-      </c>
-      <c r="B38" s="12"/>
-      <c r="C38" s="12"/>
-      <c r="D38" s="12"/>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A40" t="s">
-        <v>21</v>
-      </c>
-      <c r="B40" s="1">
-        <v>2</v>
-      </c>
-      <c r="C40" s="1">
-        <v>2</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A41" t="s">
-        <v>79</v>
-      </c>
-      <c r="B41" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A42" t="s">
-        <v>25</v>
-      </c>
-      <c r="B42" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A43" t="s">
-        <v>24</v>
-      </c>
-      <c r="B43" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A44" t="s">
-        <v>97</v>
-      </c>
-      <c r="B44" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A45" t="s">
-        <v>146</v>
-      </c>
-      <c r="B45" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A46" t="s">
-        <v>96</v>
-      </c>
-      <c r="B46" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A47" t="s">
-        <v>20</v>
-      </c>
-      <c r="B47" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A48" t="s">
-        <v>22</v>
-      </c>
-      <c r="B48" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A49" t="s">
-        <v>23</v>
-      </c>
-      <c r="B49" s="1">
-        <v>2</v>
-      </c>
-      <c r="C49" s="1">
-        <v>2</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A50" t="s">
-        <v>73</v>
-      </c>
-      <c r="B50" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A51" t="s">
-        <v>19</v>
-      </c>
-      <c r="B51" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A52" t="s">
-        <v>76</v>
-      </c>
-      <c r="B52" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A53" t="s">
-        <v>98</v>
-      </c>
-      <c r="B53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A54" t="s">
-        <v>99</v>
-      </c>
-      <c r="B54">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A55" t="s">
-        <v>100</v>
-      </c>
-      <c r="B55">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A56" t="s">
-        <v>103</v>
-      </c>
-      <c r="B56">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A57" t="s">
-        <v>104</v>
-      </c>
-      <c r="B57">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A63" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="B63" s="12"/>
-      <c r="C63" s="12"/>
-      <c r="D63" s="12"/>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A65" t="s">
-        <v>149</v>
-      </c>
-      <c r="B65" s="1">
-        <v>4</v>
-      </c>
-      <c r="C65" s="1">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A66" t="s">
-        <v>150</v>
-      </c>
-      <c r="B66" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A67" t="s">
-        <v>151</v>
-      </c>
-      <c r="B67" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A68" t="s">
-        <v>152</v>
-      </c>
-      <c r="B68" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A69" t="s">
-        <v>153</v>
-      </c>
-      <c r="B69" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A70" t="s">
-        <v>154</v>
-      </c>
-      <c r="B70" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A71" t="s">
-        <v>155</v>
-      </c>
-      <c r="B71" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A72" t="s">
-        <v>156</v>
-      </c>
-      <c r="B72" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A73" t="s">
-        <v>157</v>
-      </c>
-      <c r="B73" s="1">
-        <v>6</v>
-      </c>
-      <c r="C73" s="1">
-        <v>50</v>
-      </c>
-      <c r="D73" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A74" t="s">
-        <v>47</v>
-      </c>
-      <c r="B74" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A75" t="s">
-        <v>42</v>
-      </c>
-      <c r="B75" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A76" t="s">
-        <v>158</v>
-      </c>
-      <c r="B76" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A77" t="s">
-        <v>48</v>
-      </c>
-      <c r="B77" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B79"/>
-    </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B81"/>
-    </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B83"/>
-    </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B85"/>
-    </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B86"/>
-    </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B87"/>
-    </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B89"/>
-    </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B90"/>
-    </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B91"/>
-    </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B92"/>
-    </row>
-    <row r="93" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B93"/>
-    </row>
-    <row r="94" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B94"/>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A99" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="B99" s="12"/>
-      <c r="C99" s="12"/>
-      <c r="D99" s="12"/>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A101" t="s">
-        <v>160</v>
-      </c>
-      <c r="B101" s="1">
-        <v>1</v>
-      </c>
-      <c r="C101" s="1">
-        <v>15</v>
-      </c>
-      <c r="D101" s="1" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A102" t="s">
-        <v>168</v>
-      </c>
-      <c r="B102" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A121" s="12" t="s">
+      <c r="C114" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="D114" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="B121" s="12"/>
-      <c r="C121" s="12"/>
-      <c r="D121" s="12"/>
-    </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A123" t="s">
-        <v>164</v>
-      </c>
-      <c r="B123" s="1">
-        <v>2</v>
-      </c>
-      <c r="C123" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="D123" s="3" t="s">
+      <c r="F114">
+        <f t="shared" ref="F114:F116" si="0">B114*C114</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6">
+      <c r="A115" t="s">
         <v>165</v>
       </c>
-      <c r="F123">
-        <f>B123*C123</f>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A124" t="s">
+      <c r="B115" s="1">
+        <v>10</v>
+      </c>
+      <c r="C115" s="1">
+        <v>1</v>
+      </c>
+      <c r="D115" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="F115">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" ht="14.65" thickBot="1">
+      <c r="A116" t="s">
         <v>166</v>
       </c>
-      <c r="B124" s="1">
+      <c r="B116" s="1">
         <v>0</v>
       </c>
-      <c r="C124" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="D124" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="F124">
-        <f t="shared" ref="F124:F126" si="0">B124*C124</f>
+      <c r="C116" s="1">
+        <v>10</v>
+      </c>
+      <c r="D116" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="F116" s="16">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A125" t="s">
-        <v>161</v>
-      </c>
-      <c r="B125" s="1">
-        <v>101</v>
-      </c>
-      <c r="C125" s="1">
-        <v>1</v>
-      </c>
-      <c r="D125" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="F125">
-        <f t="shared" si="0"/>
-        <v>101</v>
-      </c>
-    </row>
-    <row r="126" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A126" t="s">
-        <v>162</v>
-      </c>
-      <c r="B126" s="1">
-        <v>20</v>
-      </c>
-      <c r="C126" s="1">
-        <v>10</v>
-      </c>
-      <c r="D126" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="F126" s="19">
-        <f t="shared" si="0"/>
-        <v>200</v>
-      </c>
-    </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="F127" s="20">
-        <f>SUM(F123:F126)</f>
-        <v>301.02</v>
+    <row r="117" spans="1:6">
+      <c r="F117" s="17">
+        <f>SUM(F113:F116)</f>
+        <v>10.02</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A101:D107">
-    <sortCondition ref="A101"/>
-  </sortState>
   <mergeCells count="7">
-    <mergeCell ref="A63:D63"/>
-    <mergeCell ref="A121:D121"/>
+    <mergeCell ref="A60:D60"/>
+    <mergeCell ref="A111:D111"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="A23:D23"/>
-    <mergeCell ref="A38:D38"/>
-    <mergeCell ref="A99:D99"/>
+    <mergeCell ref="A35:D35"/>
+    <mergeCell ref="A91:D91"/>
     <mergeCell ref="A16:D16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>